<commit_message>
refactor: optimize hazard pointer stroage handling
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/hazard_pointer.xlsx
+++ b/libalconcurrent/doc/hazard_pointer.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79D50FC-FA43-4849-934E-6F11E61B82BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F47AC6-9390-4245-B264-4E5C7B6134BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="基本構造" sheetId="1" r:id="rId1"/>
+    <sheet name="スレッド生成終了に対応するためのvalid chain" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -86,6 +87,101 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5197BE6B-F092-4E3B-85E5-6B349CCF69B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="438150" y="1657350"/>
+          <a:ext cx="4162425" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>グローバル変数</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>global_scope_hazard_ptr_chain::g_scope_valid_hzrd_chain_</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -486,6 +582,24 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPct val="100000"/>
@@ -821,6 +935,24 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPct val="100000"/>
@@ -1050,6 +1182,24 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPct val="100000"/>
@@ -1411,8 +1561,8 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -1433,8 +1583,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5153025" y="3371849"/>
-          <a:ext cx="4267200" cy="2238375"/>
+          <a:off x="5153025" y="3571875"/>
+          <a:ext cx="4267200" cy="2038349"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2346,8 +2496,8 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -2368,8 +2518,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3295650" y="3924300"/>
-          <a:ext cx="2352675" cy="2476500"/>
+          <a:off x="3295650" y="4057650"/>
+          <a:ext cx="2352675" cy="2343150"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3335,6 +3485,2598 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>200026</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="フリーフォーム: 図形 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13E90BBA-765F-4E1A-92E6-9E30DCB46049}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3181351" y="2143126"/>
+          <a:ext cx="2000250" cy="914400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 2085975"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 1828800"/>
+            <a:gd name="connsiteX1" fmla="*/ 485775 w 2085975"/>
+            <a:gd name="connsiteY1" fmla="*/ 1466850 h 1828800"/>
+            <a:gd name="connsiteX2" fmla="*/ 1371600 w 2085975"/>
+            <a:gd name="connsiteY2" fmla="*/ 1828800 h 1828800"/>
+            <a:gd name="connsiteX3" fmla="*/ 2085975 w 2085975"/>
+            <a:gd name="connsiteY3" fmla="*/ 1828800 h 1828800"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2085975" h="1828800">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="485775" y="1466850"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1371600" y="1828800"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2085975" y="1828800"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4CBE32E-4A4E-4DF5-AD70-15FAE708F894}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2895600" y="1704975"/>
+          <a:ext cx="3657601" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>class hazard_ptr_group {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>    std::atomic&lt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hazard_ptr_group*&gt; ap_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;hazard_ptr_group*&gt; ap_list_next_;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;bool&gt; is_used_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>    std::atomic&lt;void*&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>hzrd_ptr_array[32];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;void*&gt;*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> try_assign(void *p);</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>};</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{511942B3-CBCD-90D0-390B-6F6498D5C7DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="1685925"/>
+          <a:ext cx="3657601" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>class hazard_ptr_group {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    std::atomic&lt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hazard_ptr_group*&gt; ap_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;hazard_ptr_group*&gt; ap_list_next_;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;bool&gt; is_used_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    std::atomic&lt;void*&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>hzrd_ptr_array[32];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;void*&gt;*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> try_assign(void *p);</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>};</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A935AD8C-F223-8BF8-245B-9C11323884EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11982450" y="1685925"/>
+          <a:ext cx="3657601" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>class hazard_ptr_group {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    std::atomic&lt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hazard_ptr_group*&gt; ap_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;hazard_ptr_group*&gt; ap_list_next_;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;bool&gt; is_used_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    std::atomic&lt;void*&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>hzrd_ptr_array[32];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;void*&gt;*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> try_assign(void *p);</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>};</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{866E1AD8-281D-BAEA-190C-29106F94EB2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2886075" y="3790950"/>
+          <a:ext cx="3657601" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>class hazard_ptr_group {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>    std::atomic&lt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hazard_ptr_group*&gt; ap_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;hazard_ptr_group*&gt; ap_list_next_;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;bool&gt; is_used_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>    std::atomic&lt;void*&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>hzrd_ptr_array[32];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;void*&gt;*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> try_assign(void *p);</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>};</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="正方形/長方形 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20CE0B20-85D2-229C-ED13-7AA886606679}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11972925" y="3771900"/>
+          <a:ext cx="3657601" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>class hazard_ptr_group {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    std::atomic&lt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hazard_ptr_group*&gt; ap_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;hazard_ptr_group*&gt; ap_list_next_;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;bool&gt; is_used_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    std::atomic&lt;void*&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>hzrd_ptr_array[32];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;void*&gt;*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> try_assign(void *p);</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>};</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="正方形/長方形 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{316C35EB-04B0-81E4-9A3F-E4E0C5333A02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16478250" y="1685925"/>
+          <a:ext cx="3657601" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>class hazard_ptr_group {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>    std::atomic&lt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hazard_ptr_group*&gt; ap_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;std::uintptr_t&gt; aaddr_valid_chain_next_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    std::atomic&lt;hazard_ptr_group*&gt; ap_list_next_;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;bool&gt; is_used_;</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>    std::atomic&lt;void*&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>hzrd_ptr_array[32];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>std::atomic&lt;void*&gt;*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> try_assign(void *p);</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>};</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="フリーフォーム: 図形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{664D27CF-644B-FB12-B3BB-998A4DAC2FE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6010275" y="1828800"/>
+          <a:ext cx="1457325" cy="200025"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1457325"/>
+            <a:gd name="connsiteY0" fmla="*/ 200025 h 200025"/>
+            <a:gd name="connsiteX1" fmla="*/ 809625 w 1457325"/>
+            <a:gd name="connsiteY1" fmla="*/ 200025 h 200025"/>
+            <a:gd name="connsiteX2" fmla="*/ 1076325 w 1457325"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 200025"/>
+            <a:gd name="connsiteX3" fmla="*/ 1457325 w 1457325"/>
+            <a:gd name="connsiteY3" fmla="*/ 0 h 200025"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1457325" h="200025">
+              <a:moveTo>
+                <a:pt x="0" y="200025"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="809625" y="200025"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1076325" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1457325" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="フリーフォーム: 図形 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BC3BAE3-DA2C-4B0C-918A-D9F66107709C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10572750" y="1809750"/>
+          <a:ext cx="1457325" cy="200025"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1457325"/>
+            <a:gd name="connsiteY0" fmla="*/ 200025 h 200025"/>
+            <a:gd name="connsiteX1" fmla="*/ 809625 w 1457325"/>
+            <a:gd name="connsiteY1" fmla="*/ 200025 h 200025"/>
+            <a:gd name="connsiteX2" fmla="*/ 1076325 w 1457325"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 200025"/>
+            <a:gd name="connsiteX3" fmla="*/ 1457325 w 1457325"/>
+            <a:gd name="connsiteY3" fmla="*/ 0 h 200025"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1457325" h="200025">
+              <a:moveTo>
+                <a:pt x="0" y="200025"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="809625" y="200025"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1076325" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1457325" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="フリーフォーム: 図形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFAFD915-2B43-4147-A27D-0AFE880CE2AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15078075" y="1809750"/>
+          <a:ext cx="1457325" cy="200025"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1457325"/>
+            <a:gd name="connsiteY0" fmla="*/ 200025 h 200025"/>
+            <a:gd name="connsiteX1" fmla="*/ 809625 w 1457325"/>
+            <a:gd name="connsiteY1" fmla="*/ 200025 h 200025"/>
+            <a:gd name="connsiteX2" fmla="*/ 1076325 w 1457325"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 200025"/>
+            <a:gd name="connsiteX3" fmla="*/ 1457325 w 1457325"/>
+            <a:gd name="connsiteY3" fmla="*/ 0 h 200025"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1457325" h="200025">
+              <a:moveTo>
+                <a:pt x="0" y="200025"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="809625" y="200025"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1076325" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1457325" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="フリーフォーム: 図形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ED4C2CC-94B8-61E8-633D-B57400FFC616}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6353175" y="1285875"/>
+          <a:ext cx="10163175" cy="904875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 10163175"/>
+            <a:gd name="connsiteY0" fmla="*/ 904875 h 904875"/>
+            <a:gd name="connsiteX1" fmla="*/ 295275 w 10163175"/>
+            <a:gd name="connsiteY1" fmla="*/ 904875 h 904875"/>
+            <a:gd name="connsiteX2" fmla="*/ 657225 w 10163175"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 904875"/>
+            <a:gd name="connsiteX3" fmla="*/ 9629775 w 10163175"/>
+            <a:gd name="connsiteY3" fmla="*/ 0 h 904875"/>
+            <a:gd name="connsiteX4" fmla="*/ 9886950 w 10163175"/>
+            <a:gd name="connsiteY4" fmla="*/ 476250 h 904875"/>
+            <a:gd name="connsiteX5" fmla="*/ 10163175 w 10163175"/>
+            <a:gd name="connsiteY5" fmla="*/ 476250 h 904875"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="10163175" h="904875">
+              <a:moveTo>
+                <a:pt x="0" y="904875"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="295275" y="904875"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="657225" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="9629775" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="9886950" y="476250"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="10163175" y="476250"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="楕円 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C50F7E74-751F-E3F0-A8A4-83A4EDF0160B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4981575" y="4257675"/>
+          <a:ext cx="990600" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>209551</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="吹き出し: 角を丸めた四角形 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7921F6DA-033F-2CA3-8C88-DC0FB2015282}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2447925" y="1200150"/>
+          <a:ext cx="3019425" cy="1866901"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 39734"/>
+            <a:gd name="adj2" fmla="val 111613"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>この変数によるリスト構造は常に有効。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>存在する</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>hazard_ptr_group</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>のすべてにつながるリンク。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>空き</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>hazard_ptr_group</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>を見つけるときは、このリンクをたどることで見つけることができる。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="楕円 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6924AB3-040A-4E5A-845A-B94936402FAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="4486275"/>
+          <a:ext cx="1333500" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>219076</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19052</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="吹き出し: 角を丸めた四角形 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDDF6621-FF9B-44CE-AC85-23F96730441C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6991349" y="6410326"/>
+          <a:ext cx="6448425" cy="2657476"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -65113"/>
+            <a:gd name="adj2" fmla="val -115374"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>この変数によるリスト構造は、スレッドと紐づいている</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>hazard_ptr_group</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>のすべてにつながるリンク。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>hazard_ptr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>かどうかチェックするときに、このリンクをたどって、チェックする。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>なお、この変数は</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hazard_ptr_group</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>が</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>スレッドから切り離されても値を維持する。これは、別スレッドがこの</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hazard_ptr_group</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>を</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>観測中に無効化されても、リンクをたどって処理を継続できるようにするため。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>また、最有効化時には、この辺巣のリンクの先頭に移動させる。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>先頭に移動したことによって、再チェックの無駄が発生するが、処理自体は継続し、ハザードポインタチェックも正常に行われる。</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3608,8 +6350,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAFF6D9-14B0-4B3A-B016-6E17AB7CD06A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>